<commit_message>
word extracted from excel ;-(
</commit_message>
<xml_diff>
--- a/_work/HTML-tags.xlsx
+++ b/_work/HTML-tags.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tags" sheetId="1" r:id="rId1"/>
     <sheet name="XHTML1-Strict Entity list" sheetId="5" r:id="rId2"/>
     <sheet name="HTML4 Attributes" sheetId="4" r:id="rId3"/>
-    <sheet name="HTML5 - Kinds of content " sheetId="2" r:id="rId4"/>
-    <sheet name="Resources" sheetId="3" r:id="rId5"/>
-    <sheet name="Display comparison" sheetId="6" r:id="rId6"/>
+    <sheet name="Resources" sheetId="3" r:id="rId4"/>
+    <sheet name="Display comparison" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tags!$B$2:$AF$2</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -4589,14 +4588,14 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4612,52 +4611,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
-          <xdr:row>0</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>66675</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Object 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4949,7 +4902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -4970,22 +4923,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="61" t="s">
         <v>164</v>
       </c>
-      <c r="H1" s="60"/>
-      <c r="I1" s="61" t="s">
+      <c r="H1" s="61"/>
+      <c r="I1" s="62" t="s">
         <v>156</v>
       </c>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
       <c r="S1" s="22"/>
       <c r="T1" s="22"/>
       <c r="U1" s="22"/>
@@ -5379,7 +5332,7 @@
         <f t="shared" si="0"/>
         <v>article</v>
       </c>
-      <c r="E9" s="62" t="s">
+      <c r="E9" s="60" t="s">
         <v>912</v>
       </c>
       <c r="F9" t="s">
@@ -5428,7 +5381,7 @@
         <f t="shared" si="0"/>
         <v>aside</v>
       </c>
-      <c r="E10" s="62" t="s">
+      <c r="E10" s="60" t="s">
         <v>912</v>
       </c>
       <c r="F10" t="s">
@@ -5785,7 +5738,7 @@
         <f t="shared" si="1"/>
         <v>blockquote</v>
       </c>
-      <c r="E18" s="62" t="s">
+      <c r="E18" s="60" t="s">
         <v>910</v>
       </c>
       <c r="F18" s="3" t="s">
@@ -5832,7 +5785,7 @@
         <f t="shared" si="1"/>
         <v>body</v>
       </c>
-      <c r="E19" s="62" t="s">
+      <c r="E19" s="60" t="s">
         <v>910</v>
       </c>
       <c r="F19" s="3"/>
@@ -6437,7 +6390,7 @@
         <f t="shared" si="1"/>
         <v>details</v>
       </c>
-      <c r="E33" s="62" t="s">
+      <c r="E33" s="60" t="s">
         <v>910</v>
       </c>
       <c r="F33" t="s">
@@ -6825,7 +6778,7 @@
         <f t="shared" ref="D42:D71" si="2">HYPERLINK(CONCATENATE("https://developer.mozilla.org/en/HTML/Element/", A42), A42)</f>
         <v>fieldset</v>
       </c>
-      <c r="E42" s="62" t="s">
+      <c r="E42" s="60" t="s">
         <v>910</v>
       </c>
       <c r="F42" s="3"/>
@@ -6909,7 +6862,7 @@
         <f t="shared" si="2"/>
         <v>figure</v>
       </c>
-      <c r="E44" s="62" t="s">
+      <c r="E44" s="60" t="s">
         <v>910</v>
       </c>
       <c r="F44" t="s">
@@ -8308,7 +8261,7 @@
         <f>HYPERLINK(CONCATENATE("https://developer.mozilla.org/en/HTML/Element/", A76), A76)</f>
         <v>nav</v>
       </c>
-      <c r="E76" s="62" t="s">
+      <c r="E76" s="60" t="s">
         <v>912</v>
       </c>
       <c r="F76" t="s">
@@ -9203,7 +9156,7 @@
         <f t="shared" si="3"/>
         <v>section</v>
       </c>
-      <c r="E97" s="62" t="s">
+      <c r="E97" s="60" t="s">
         <v>912</v>
       </c>
       <c r="F97" t="s">
@@ -9807,7 +9760,7 @@
         <f t="shared" si="5"/>
         <v>td</v>
       </c>
-      <c r="E111" s="62" t="s">
+      <c r="E111" s="60" t="s">
         <v>910</v>
       </c>
       <c r="F111" s="3"/>
@@ -14987,51 +14940,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-  <oleObjects>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="Document" dvAspect="DVASPECT_ICON" shapeId="1025" r:id="rId3">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId4">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>66675</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="Document" dvAspect="DVASPECT_ICON" shapeId="1025" r:id="rId3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-  </oleObjects>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -15100,7 +15012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H30"/>
   <sheetViews>

</xml_diff>